<commit_message>
updated planning & design
</commit_message>
<xml_diff>
--- a/CST-235 Burndown Chart.xlsx
+++ b/CST-235 Burndown Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poker\Documents\CST-235\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poker\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CF97FE-2E34-4A5A-8918-0FDA9E784BDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D67C90-2BA2-4AA1-91A3-569BF3226E31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -670,19 +670,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -818,37 +818,37 @@
                   <c:v>57.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.045454545454547</c:v>
+                  <c:v>51.045454545454547</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.590909090909093</c:v>
+                  <c:v>45.090909090909093</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.13636363636364</c:v>
+                  <c:v>40.13636363636364</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.681818181818187</c:v>
+                  <c:v>35.681818181818187</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.227272727272732</c:v>
+                  <c:v>28.227272727272734</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.77272727272727693</c:v>
+                  <c:v>17.77272727272728</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-9.6818181818181781</c:v>
+                  <c:v>7.3181818181818254</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-20.136363636363633</c:v>
+                  <c:v>-3.1363636363636296</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-30.590909090909086</c:v>
+                  <c:v>-13.590909090909085</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-41.04545454545454</c:v>
+                  <c:v>-24.04545454545454</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-51.499999999999993</c:v>
+                  <c:v>-34.499999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2145,8 +2145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23A665-88C7-4222-B918-AB1BED6AEF55}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2217,7 +2217,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" s="19">
         <v>0</v>
@@ -2262,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="21">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E3" s="21">
         <v>0</v>
@@ -2307,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="19">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="F4" s="19">
         <v>0</v>
@@ -2352,7 +2352,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="21">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G5" s="21">
         <v>0</v>
@@ -2397,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="20">
         <v>0</v>
@@ -2777,23 +2777,23 @@
       <c r="B20" s="8"/>
       <c r="C20" s="8">
         <f>SUM(C2:C12)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="8">
         <f t="shared" ref="D20:M20" si="1">SUM(D2:D12)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E20" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="F20" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G20" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20" s="8">
         <f t="shared" si="1"/>
@@ -2830,47 +2830,47 @@
       </c>
       <c r="C21" s="6">
         <f>IF(C20 &gt;= C19, B21-C19+(C20-C19), B21-(C19+(C19-C20)))</f>
-        <v>53.045454545454547</v>
+        <v>51.045454545454547</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" ref="D21:M21" si="2">IF(D20 &gt;= D19, C21-D19+(D20-D19), C21-(D19+(D19-D20)))</f>
-        <v>42.590909090909093</v>
+        <v>45.090909090909093</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" si="2"/>
-        <v>32.13636363636364</v>
+        <v>40.13636363636364</v>
       </c>
       <c r="F21" s="6">
         <f t="shared" si="2"/>
-        <v>21.681818181818187</v>
+        <v>35.681818181818187</v>
       </c>
       <c r="G21" s="6">
         <f t="shared" si="2"/>
-        <v>11.227272727272732</v>
+        <v>28.227272727272734</v>
       </c>
       <c r="H21" s="6">
         <f t="shared" si="2"/>
-        <v>0.77272727272727693</v>
+        <v>17.77272727272728</v>
       </c>
       <c r="I21" s="6">
         <f t="shared" si="2"/>
-        <v>-9.6818181818181781</v>
+        <v>7.3181818181818254</v>
       </c>
       <c r="J21" s="6">
         <f t="shared" si="2"/>
-        <v>-20.136363636363633</v>
+        <v>-3.1363636363636296</v>
       </c>
       <c r="K21" s="6">
         <f t="shared" si="2"/>
-        <v>-30.590909090909086</v>
+        <v>-13.590909090909085</v>
       </c>
       <c r="L21" s="6">
         <f t="shared" si="2"/>
-        <v>-41.04545454545454</v>
+        <v>-24.04545454545454</v>
       </c>
       <c r="M21" s="6">
         <f t="shared" si="2"/>
-        <v>-51.499999999999993</v>
+        <v>-34.499999999999993</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>